<commit_message>
Basic scales (no modes or variations).
</commit_message>
<xml_diff>
--- a/src/math.xlsx
+++ b/src/math.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marten\Code\Waves\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3AEC335-5A6A-47BA-9D4F-47DA0382C18C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{809B70D4-AA32-42B8-BF4A-4AA6B5776E17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2565" yWindow="7860" windowWidth="15855" windowHeight="21900" xr2:uid="{1F8B8F39-28C3-4355-AAAB-7FA9C73974E0}"/>
+    <workbookView xWindow="9945" yWindow="9960" windowWidth="20625" windowHeight="22440" activeTab="2" xr2:uid="{1F8B8F39-28C3-4355-AAAB-7FA9C73974E0}"/>
   </bookViews>
   <sheets>
     <sheet name="tuning" sheetId="2" r:id="rId1"/>
     <sheet name="exponential" sheetId="1" r:id="rId2"/>
+    <sheet name="scales" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>gain</t>
   </si>
@@ -93,18 +94,91 @@
   <si>
     <t xml:space="preserve"> </t>
   </si>
+  <si>
+    <t>chromatic</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>C#</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>D#</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>F#</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>G#</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>A#</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>octatonic</t>
+  </si>
+  <si>
+    <t>heptatonic</t>
+  </si>
+  <si>
+    <t>hexatonic</t>
+  </si>
+  <si>
+    <t>pentatonic</t>
+  </si>
+  <si>
+    <t>tetratonic</t>
+  </si>
+  <si>
+    <t>tritonic</t>
+  </si>
+  <si>
+    <t>ditonic</t>
+  </si>
+  <si>
+    <t>monotonic</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -139,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -147,10 +221,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1898,8 +1981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB0363C9-2C87-4851-AD47-0926EAD643CE}">
   <dimension ref="B3:L114"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1979,7 +2062,7 @@
         <v>464</v>
       </c>
       <c r="G6">
-        <f t="shared" ref="G6:G66" si="1">G5+1</f>
+        <f t="shared" ref="G6:G63" si="1">G5+1</f>
         <v>26</v>
       </c>
       <c r="H6" s="4">
@@ -3236,11 +3319,11 @@
         <v>6</v>
       </c>
       <c r="G112">
-        <f t="shared" ref="G112:G114" si="6">G111+1</f>
+        <f t="shared" ref="G112" si="6">G111+1</f>
         <v>132</v>
       </c>
       <c r="H112" s="4">
-        <f t="shared" ref="H112:H114" si="7">2^((G112-69)/12)*440</f>
+        <f t="shared" ref="H112" si="7">2^((G112-69)/12)*440</f>
         <v>16744.036179238312</v>
       </c>
     </row>
@@ -3880,4 +3963,765 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08C38BFC-EC36-457C-99C7-5CF42FD25833}">
+  <dimension ref="B4:K31"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="11" width="10.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="6">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="6">
+        <f>B5</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="6">
+        <f>B5</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="6">
+        <f>B5</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="6">
+        <f>B5</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="6">
+        <f>B5</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="6">
+        <f>B5</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="6">
+        <f>B5</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="6">
+        <f>B5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="6">
+        <v>2</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="6">
+        <f>B7</f>
+        <v>2</v>
+      </c>
+      <c r="E7" s="6">
+        <f>B7</f>
+        <v>2</v>
+      </c>
+      <c r="F7" s="6">
+        <f>B7</f>
+        <v>2</v>
+      </c>
+      <c r="G7" s="6">
+        <f>B7</f>
+        <v>2</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="6">
+        <v>3</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="6">
+        <f>B8</f>
+        <v>3</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6">
+        <f>B8</f>
+        <v>3</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="6">
+        <v>4</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6">
+        <f>B9</f>
+        <v>4</v>
+      </c>
+      <c r="F9" s="6">
+        <f>B9</f>
+        <v>4</v>
+      </c>
+      <c r="G9" s="6">
+        <f>B9</f>
+        <v>4</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6">
+        <f>B9</f>
+        <v>4</v>
+      </c>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="6">
+        <v>5</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="6">
+        <f>B10</f>
+        <v>5</v>
+      </c>
+      <c r="E10" s="6">
+        <f>B10</f>
+        <v>5</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="6">
+        <v>6</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="6">
+        <f>B11</f>
+        <v>6</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6">
+        <f>B11</f>
+        <v>6</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6">
+        <f>B11</f>
+        <v>6</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6">
+        <f>B11</f>
+        <v>6</v>
+      </c>
+      <c r="K11" s="6"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="6">
+        <v>7</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6">
+        <f>B12</f>
+        <v>7</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6">
+        <f>B12</f>
+        <v>7</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="6">
+        <v>8</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="6">
+        <f>B13</f>
+        <v>8</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6">
+        <f>B13</f>
+        <v>8</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6">
+        <f>B13</f>
+        <v>8</v>
+      </c>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="6">
+        <v>9</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="6">
+        <f>B14</f>
+        <v>9</v>
+      </c>
+      <c r="E14" s="6">
+        <f>B14</f>
+        <v>9</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6">
+        <f>B14</f>
+        <v>9</v>
+      </c>
+      <c r="H14" s="6">
+        <f>B14</f>
+        <v>9</v>
+      </c>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="6">
+        <v>10</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6">
+        <f>B15</f>
+        <v>10</v>
+      </c>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="6">
+        <v>11</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="6">
+        <f>B16</f>
+        <v>11</v>
+      </c>
+      <c r="E16" s="6">
+        <f>B16</f>
+        <v>11</v>
+      </c>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+    </row>
+    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D19" s="6">
+        <f>IF(D5&lt;&gt;"",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E19" s="6">
+        <f t="shared" ref="E19:K19" si="0">IF(E5&lt;&gt;"",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F19" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G19" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H19" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I19" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J19" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K19" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D20" s="6">
+        <f t="shared" ref="D20:K31" si="1">IF(D6&lt;&gt;"",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K20" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D21" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E21" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F21" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G21" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H21" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K21" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D22" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E22" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I22" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K22" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D23" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E23" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F23" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G23" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H23" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J23" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D24" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E24" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F24" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D25" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E25" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G25" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H25" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I25" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J25" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K25" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D26" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E26" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F26" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H26" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J26" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K26" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D27" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E27" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G27" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H27" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I27" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J27" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K27" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D28" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E28" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F28" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G28" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H28" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I28" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J28" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K28" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D29" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E29" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G29" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H29" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I29" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J29" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K29" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D30" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E30" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F30" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G30" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H30" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I30" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J30" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K30" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D31" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>